<commit_message>
many tests at one time
</commit_message>
<xml_diff>
--- a/local vs global/Default.xlsx
+++ b/local vs global/Default.xlsx
@@ -510,7 +510,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -563,7 +563,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>

</xml_diff>